<commit_message>
modified and added examples
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="154">
   <si>
     <t>Topic</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>What is Functional Interface?</t>
-  </si>
-  <si>
-    <t>Can we create more than one method inside Functional Interface?</t>
   </si>
   <si>
     <t>What is Lambda Function?</t>
@@ -468,6 +465,21 @@
   </si>
   <si>
     <t>What is the size of boolean, byte, sort, char, int, float, long and double primitive data types?</t>
+  </si>
+  <si>
+    <t>https://medium.com/@itsromiljain/curious-case-of-concurrenthashmap-90249632d335</t>
+  </si>
+  <si>
+    <t>Can we create more than one abstract method inside Functional Interface?</t>
+  </si>
+  <si>
+    <t>http://www.instanceofjava.com/2016/08/final-static-method-in-java-example.html</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Context_switch</t>
+  </si>
+  <si>
+    <t>https://howtodoinjava.com/java/multi-threading/executor-framework-tutorial/</t>
   </si>
 </sst>
 </file>
@@ -1345,8 +1357,8 @@
   <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1376,7 +1388,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
@@ -1387,7 +1399,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1398,7 +1410,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1469,10 +1481,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1491,7 +1503,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30">
@@ -1502,7 +1514,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1518,7 +1530,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1537,17 +1549,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" ht="30">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>31</v>
@@ -1555,59 +1570,59 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30">
+      <c r="A24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>79</v>
+      <c r="C24" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1615,7 +1630,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1623,7 +1638,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="75">
@@ -1631,42 +1646,42 @@
         <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1674,7 +1689,10 @@
         <v>24</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1682,7 +1700,7 @@
         <v>24</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1690,7 +1708,7 @@
         <v>24</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1698,7 +1716,7 @@
         <v>24</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30">
@@ -1706,7 +1724,7 @@
         <v>24</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1714,7 +1732,7 @@
         <v>24</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1722,7 +1740,7 @@
         <v>24</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1730,7 +1748,7 @@
         <v>24</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1738,7 +1756,7 @@
         <v>24</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1746,10 +1764,10 @@
         <v>24</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1757,7 +1775,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30">
@@ -1765,10 +1783,10 @@
         <v>3</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30">
@@ -1776,10 +1794,10 @@
         <v>27</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1787,7 +1805,7 @@
         <v>24</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30">
@@ -1795,10 +1813,10 @@
         <v>24</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1806,7 +1824,7 @@
         <v>24</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1814,7 +1832,7 @@
         <v>24</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1822,7 +1840,7 @@
         <v>24</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30">
@@ -1830,10 +1848,10 @@
         <v>24</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="30">
@@ -1841,10 +1859,10 @@
         <v>24</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="30">
@@ -1852,10 +1870,10 @@
         <v>24</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1863,10 +1881,10 @@
         <v>24</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1874,7 +1892,7 @@
         <v>24</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1882,7 +1900,7 @@
         <v>24</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="30">
@@ -1890,10 +1908,10 @@
         <v>8</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1901,7 +1919,7 @@
         <v>24</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1909,7 +1927,7 @@
         <v>24</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1917,15 +1935,18 @@
         <v>24</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30">
+      <c r="A62" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>88</v>
+      <c r="C62" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="45">
@@ -1933,10 +1954,10 @@
         <v>24</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="30">
@@ -1944,7 +1965,7 @@
         <v>24</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1952,18 +1973,18 @@
         <v>24</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="30">
       <c r="A66" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1971,7 +1992,7 @@
         <v>24</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1979,7 +2000,7 @@
         <v>24</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="45">
@@ -1987,10 +2008,10 @@
         <v>24</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="30">
@@ -1998,32 +2019,32 @@
         <v>27</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="30">
       <c r="A71" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2031,7 +2052,7 @@
         <v>27</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2039,18 +2060,18 @@
         <v>27</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="30">
       <c r="A75" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="30">
@@ -2058,10 +2079,10 @@
         <v>27</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2069,7 +2090,7 @@
         <v>27</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2077,7 +2098,7 @@
         <v>27</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="45">
@@ -2085,10 +2106,10 @@
         <v>27</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="45">
@@ -2096,10 +2117,10 @@
         <v>27</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="30">
@@ -2107,10 +2128,10 @@
         <v>27</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="30">
@@ -2118,10 +2139,10 @@
         <v>27</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="30">
@@ -2129,10 +2150,10 @@
         <v>27</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="30">
@@ -2140,10 +2161,10 @@
         <v>27</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="30">
@@ -2151,10 +2172,10 @@
         <v>27</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="30">
@@ -2162,10 +2183,10 @@
         <v>24</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2173,7 +2194,7 @@
         <v>24</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2181,82 +2202,82 @@
         <v>24</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="30">
       <c r="A96" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2296,8 +2317,12 @@
     <hyperlink ref="C10" r:id="rId29"/>
     <hyperlink ref="C86" r:id="rId30"/>
     <hyperlink ref="C96" r:id="rId31"/>
+    <hyperlink ref="C19" r:id="rId32"/>
+    <hyperlink ref="C24" r:id="rId33"/>
+    <hyperlink ref="C34" r:id="rId34"/>
+    <hyperlink ref="C62" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added answer link for interview question
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="155">
   <si>
     <t>Topic</t>
   </si>
@@ -480,6 +480,9 @@
   </si>
   <si>
     <t>https://howtodoinjava.com/java/multi-threading/executor-framework-tutorial/</t>
+  </si>
+  <si>
+    <t>http://karunsubramanian.com/websphere/one-important-change-in-memory-management-in-java-8/</t>
   </si>
 </sst>
 </file>
@@ -1358,7 +1361,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2253,12 +2256,15 @@
         <v>140</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" ht="30">
       <c r="A95" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>141</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="30">
@@ -2321,8 +2327,9 @@
     <hyperlink ref="C24" r:id="rId33"/>
     <hyperlink ref="C34" r:id="rId34"/>
     <hyperlink ref="C62" r:id="rId35"/>
+    <hyperlink ref="C95" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Added answer link for interview question"
This reverts commit aa157188f21254439e80394ae18858d71ca03fc6.

reverted the last commit which is not needed
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="154">
   <si>
     <t>Topic</t>
   </si>
@@ -480,9 +480,6 @@
   </si>
   <si>
     <t>https://howtodoinjava.com/java/multi-threading/executor-framework-tutorial/</t>
-  </si>
-  <si>
-    <t>http://karunsubramanian.com/websphere/one-important-change-in-memory-management-in-java-8/</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1358,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2256,15 +2253,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="30">
+    <row r="95" spans="1:3">
       <c r="A95" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="30">
@@ -2327,9 +2321,8 @@
     <hyperlink ref="C24" r:id="rId33"/>
     <hyperlink ref="C34" r:id="rId34"/>
     <hyperlink ref="C62" r:id="rId35"/>
-    <hyperlink ref="C95" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added answer link for perm gen vs metaspace
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="155">
   <si>
     <t>Topic</t>
   </si>
@@ -480,6 +480,9 @@
   </si>
   <si>
     <t>https://howtodoinjava.com/java/multi-threading/executor-framework-tutorial/</t>
+  </si>
+  <si>
+    <t>http://karunsubramanian.com/websphere/one-important-change-in-memory-management-in-java-8/</t>
   </si>
 </sst>
 </file>
@@ -1358,7 +1361,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2253,12 +2256,15 @@
         <v>140</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" ht="30">
       <c r="A95" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>141</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="30">
@@ -2321,8 +2327,9 @@
     <hyperlink ref="C24" r:id="rId33"/>
     <hyperlink ref="C34" r:id="rId34"/>
     <hyperlink ref="C62" r:id="rId35"/>
+    <hyperlink ref="C95" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new interview questions and added example for flatmap
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
@@ -10,14 +10,14 @@
     <sheet name="CoreJavaTopicsOrQuestions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CoreJavaTopicsOrQuestions!$A$1:$C$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CoreJavaTopicsOrQuestions!$A$1:$C$101</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="163">
   <si>
     <t>Topic</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Answers</t>
   </si>
   <si>
-    <t>Advanced</t>
-  </si>
-  <si>
     <t>How class loader works?</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
   </si>
   <si>
     <t>What is ThreadLocal?</t>
-  </si>
-  <si>
-    <t>How Java works?</t>
   </si>
   <si>
     <t>https://javarevisited.blogspot.com/2012/12/how-classloader-works-in-java.html</t>
@@ -431,9 +425,6 @@
     <t>What is the difference between PermGenSpace and MetaSpace?</t>
   </si>
   <si>
-    <t>Java8 (Advanced)</t>
-  </si>
-  <si>
     <t>What is Consumer in java?</t>
   </si>
   <si>
@@ -465,9 +456,6 @@
   </si>
   <si>
     <t>http://karunsubramanian.com/websphere/one-important-change-in-memory-management-in-java-8/</t>
-  </si>
-  <si>
-    <t>How JVM works?</t>
   </si>
   <si>
     <t>Size of the boolean in java is virtual machine dependent.
@@ -490,6 +478,36 @@
   </si>
   <si>
     <t>Stream</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/green-vs-native-threads-and-deprecated-methods-in-java/</t>
+  </si>
+  <si>
+    <t>What is shut down hook?</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/jvm-shutdown-hook-java/</t>
+  </si>
+  <si>
+    <t>What are the limitation of future interface?</t>
+  </si>
+  <si>
+    <t>https://www.javatpoint.com/completablefuture-in-java</t>
+  </si>
+  <si>
+    <t>What is CompletableFuture?</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/39472061/executorservice-submittask-vs-completablefuture-supplyasynctask-executor</t>
+  </si>
+  <si>
+    <t>JVM architechture.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dncpVFP1JeQ</t>
+  </si>
+  <si>
+    <t>Exception</t>
   </si>
 </sst>
 </file>
@@ -1364,11 +1382,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1392,43 +1410,43 @@
     </row>
     <row r="2" spans="1:3" ht="30">
       <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -1436,21 +1454,21 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>255</v>
@@ -1458,404 +1476,407 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
       <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30">
       <c r="A13" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30">
       <c r="A14" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="75">
       <c r="A29" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30">
       <c r="A38" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="30">
       <c r="A44" s="2" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30">
       <c r="A45" s="2" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="30">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="30">
+      <c r="A47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="30">
+    <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30">
+      <c r="A51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30">
       <c r="A52" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>67</v>
@@ -1866,156 +1887,159 @@
     </row>
     <row r="53" spans="1:3" ht="30">
       <c r="A53" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="30">
-      <c r="A54" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30">
+      <c r="A57" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="30">
       <c r="A58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" ht="30">
       <c r="A61" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="45">
+      <c r="A62" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="30">
-      <c r="A62" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30">
+      <c r="A63" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="45">
-      <c r="A63" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="30">
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" ht="30">
       <c r="A65" s="2" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="30">
+        <v>97</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
-        <v>155</v>
+        <v>19</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="45">
+      <c r="A68" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="45">
+    <row r="69" spans="1:3" ht="30">
       <c r="A69" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>92</v>
@@ -2026,56 +2050,56 @@
     </row>
     <row r="70" spans="1:3" ht="30">
       <c r="A70" s="2" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="30">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="2" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="2" t="s">
-        <v>156</v>
+        <v>22</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="30">
+      <c r="A74" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="30">
       <c r="A75" s="2" t="s">
-        <v>156</v>
+        <v>22</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>105</v>
@@ -2084,58 +2108,58 @@
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="30">
+    <row r="76" spans="1:3">
       <c r="A76" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="45">
+      <c r="A78" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>110</v>
+      <c r="C78" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="45">
       <c r="A79" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C79" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="30">
+      <c r="A80" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="45">
-      <c r="A80" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="30">
       <c r="A81" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>116</v>
@@ -2146,7 +2170,7 @@
     </row>
     <row r="82" spans="1:3" ht="30">
       <c r="A82" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>118</v>
@@ -2157,7 +2181,7 @@
     </row>
     <row r="83" spans="1:3" ht="30">
       <c r="A83" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>120</v>
@@ -2168,7 +2192,7 @@
     </row>
     <row r="84" spans="1:3" ht="30">
       <c r="A84" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>122</v>
@@ -2179,141 +2203,169 @@
     </row>
     <row r="85" spans="1:3" ht="30">
       <c r="A85" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="30">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="45">
       <c r="A86" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="2" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="2" t="s">
-        <v>155</v>
+        <v>86</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="2" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30">
+      <c r="A94" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>135</v>
+      <c r="C94" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="30">
       <c r="A95" s="2" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="30">
+    </row>
+    <row r="96" spans="1:3" ht="45">
       <c r="A96" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C96" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="45">
+      <c r="C96" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="2" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>150</v>
+        <v>160</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="2" t="s">
-        <v>3</v>
+        <v>147</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="2" t="s">
-        <v>151</v>
+        <v>19</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C99">
+  <autoFilter ref="A1:C101">
     <filterColumn colId="0"/>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
@@ -2322,42 +2374,48 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C45" r:id="rId3"/>
+    <hyperlink ref="C44" r:id="rId3"/>
     <hyperlink ref="C43" r:id="rId4"/>
-    <hyperlink ref="C48" r:id="rId5"/>
+    <hyperlink ref="C47" r:id="rId5"/>
     <hyperlink ref="C14" r:id="rId6"/>
     <hyperlink ref="C13" r:id="rId7"/>
-    <hyperlink ref="C52" r:id="rId8"/>
-    <hyperlink ref="C53" r:id="rId9"/>
-    <hyperlink ref="C54" r:id="rId10"/>
-    <hyperlink ref="C58" r:id="rId11"/>
-    <hyperlink ref="C63" r:id="rId12"/>
-    <hyperlink ref="C69" r:id="rId13"/>
-    <hyperlink ref="C70" r:id="rId14"/>
-    <hyperlink ref="C71" r:id="rId15"/>
-    <hyperlink ref="C66" r:id="rId16"/>
-    <hyperlink ref="C72" r:id="rId17"/>
-    <hyperlink ref="C75" r:id="rId18"/>
-    <hyperlink ref="C76" r:id="rId19"/>
-    <hyperlink ref="C80" r:id="rId20"/>
-    <hyperlink ref="C46" r:id="rId21"/>
-    <hyperlink ref="C79" r:id="rId22"/>
-    <hyperlink ref="C81" r:id="rId23"/>
-    <hyperlink ref="C82" r:id="rId24"/>
-    <hyperlink ref="C83" r:id="rId25"/>
-    <hyperlink ref="C84" r:id="rId26"/>
-    <hyperlink ref="C85" r:id="rId27"/>
+    <hyperlink ref="C51" r:id="rId8"/>
+    <hyperlink ref="C52" r:id="rId9"/>
+    <hyperlink ref="C53" r:id="rId10"/>
+    <hyperlink ref="C57" r:id="rId11"/>
+    <hyperlink ref="C62" r:id="rId12"/>
+    <hyperlink ref="C68" r:id="rId13"/>
+    <hyperlink ref="C69" r:id="rId14"/>
+    <hyperlink ref="C70" r:id="rId15"/>
+    <hyperlink ref="C65" r:id="rId16"/>
+    <hyperlink ref="C71" r:id="rId17"/>
+    <hyperlink ref="C74" r:id="rId18"/>
+    <hyperlink ref="C75" r:id="rId19"/>
+    <hyperlink ref="C79" r:id="rId20"/>
+    <hyperlink ref="C45" r:id="rId21"/>
+    <hyperlink ref="C78" r:id="rId22"/>
+    <hyperlink ref="C80" r:id="rId23"/>
+    <hyperlink ref="C81" r:id="rId24"/>
+    <hyperlink ref="C82" r:id="rId25"/>
+    <hyperlink ref="C83" r:id="rId26"/>
+    <hyperlink ref="C84" r:id="rId27"/>
     <hyperlink ref="C11" r:id="rId28"/>
     <hyperlink ref="C10" r:id="rId29"/>
-    <hyperlink ref="C86" r:id="rId30"/>
-    <hyperlink ref="C96" r:id="rId31"/>
+    <hyperlink ref="C85" r:id="rId30"/>
+    <hyperlink ref="C95" r:id="rId31"/>
     <hyperlink ref="C19" r:id="rId32"/>
     <hyperlink ref="C24" r:id="rId33"/>
     <hyperlink ref="C34" r:id="rId34"/>
-    <hyperlink ref="C62" r:id="rId35"/>
-    <hyperlink ref="C95" r:id="rId36"/>
+    <hyperlink ref="C61" r:id="rId35"/>
+    <hyperlink ref="C94" r:id="rId36"/>
+    <hyperlink ref="C58" r:id="rId37"/>
+    <hyperlink ref="C99" r:id="rId38"/>
+    <hyperlink ref="C100" r:id="rId39"/>
+    <hyperlink ref="C101" r:id="rId40"/>
+    <hyperlink ref="C86" r:id="rId41"/>
+    <hyperlink ref="C97" r:id="rId42"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more core java interview questions and links to the answer
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
@@ -10,14 +10,14 @@
     <sheet name="CoreJavaTopicsOrQuestions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CoreJavaTopicsOrQuestions!$A$1:$C$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CoreJavaTopicsOrQuestions!$A$1:$C$104</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="179">
   <si>
     <t>Topic</t>
   </si>
@@ -508,6 +508,54 @@
   </si>
   <si>
     <t>Exception</t>
+  </si>
+  <si>
+    <t>What is Phaser?</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=J3QZ5gfCtAg</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/60159153/completablefuture-runasync-vs-supplyasync-when-to-choose-one-over-the-other</t>
+  </si>
+  <si>
+    <t>Why we need rehashing of key to find the index of hash map ?</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/40950346/hash-implementation-in-java</t>
+  </si>
+  <si>
+    <t>What is ForkJoinPool?</t>
+  </si>
+  <si>
+    <t>http://tutorials.jenkov.com/java-util-concurrent/java-fork-and-join-forkjoinpool.html</t>
+  </si>
+  <si>
+    <t>Why enum singleton is better?</t>
+  </si>
+  <si>
+    <t>https://javarevisited.blogspot.com/2012/07/why-enum-singleton-are-better-in-java.html</t>
+  </si>
+  <si>
+    <t>Why constant pool is required?</t>
+  </si>
+  <si>
+    <t>What is the use of Blocking queue?</t>
+  </si>
+  <si>
+    <t>What is the use of Priority queue?</t>
+  </si>
+  <si>
+    <t>When to use ArrayBlockingQueue, LinkedBlockingQueue and PriorityBlockingQueue?</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/7/docs/api/java/util/concurrent/BlockingQueue.html</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/17840397/concept-behind-putting-wait-notify-methods-in-object-class#:~:text=wait%20%2D%20wait%20method%20tells%20the,monitor%20and%20go%20to%20sleep.&amp;text=That's%20one%20reason%20why%20these,waiting%20on%20the%20Object's%20monitor.</t>
+  </si>
+  <si>
+    <t>Let say we locked one object thinking to so some operation and before starting the operation we found the condition is not satisfying to do that operation so as we know wait() method releases the lock. If we do not hold any lock then how can we release the lock? And if that condition satisfies then we cand easily do that operation and release the lock and notify other waiting threads that I am done with the operation now you can take a lock by calling notify() or notifyAll() method.</t>
   </si>
 </sst>
 </file>
@@ -1382,11 +1430,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1539,26 +1587,29 @@
         <v>149</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30">
+      <c r="A15" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1566,34 +1617,34 @@
         <v>149</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>149</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1601,64 +1652,64 @@
         <v>150</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>141</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30">
+      <c r="A25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1666,26 +1717,26 @@
         <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="75">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:3" ht="75">
+      <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1693,7 +1744,7 @@
         <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1701,7 +1752,7 @@
         <v>35</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1709,18 +1760,15 @@
         <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1728,7 +1776,10 @@
         <v>19</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1736,7 +1787,7 @@
         <v>19</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1744,23 +1795,29 @@
         <v>19</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="90">
+      <c r="A38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="30">
-      <c r="A38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="135">
+      <c r="A39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>45</v>
+      <c r="C39" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1768,7 +1825,7 @@
         <v>19</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1776,7 +1833,7 @@
         <v>19</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1784,7 +1841,7 @@
         <v>19</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1792,59 +1849,59 @@
         <v>19</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="30">
-      <c r="A44" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30">
       <c r="A45" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30">
+      <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="2" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="30">
-      <c r="A47" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="2" t="s">
+    <row r="48" spans="1:3" ht="30">
+      <c r="A48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1852,7 +1909,7 @@
         <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1860,18 +1917,15 @@
         <v>19</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="30">
-      <c r="A51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30">
@@ -1879,10 +1933,10 @@
         <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="30">
@@ -1890,21 +1944,21 @@
         <v>19</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30">
+      <c r="A54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1912,7 +1966,10 @@
         <v>19</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1920,67 +1977,61 @@
         <v>19</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="30">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:3">
+      <c r="A58" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30">
+      <c r="A59" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="30">
-      <c r="A58" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="2" t="s">
+    <row r="60" spans="1:3" ht="30">
+      <c r="A60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="2" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="2" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="30">
-      <c r="A61" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="45">
-      <c r="A62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="30">
@@ -1988,26 +2039,29 @@
         <v>19</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>80</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="45">
       <c r="A64" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="30">
       <c r="A65" s="2" t="s">
-        <v>151</v>
+        <v>19</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2015,157 +2069,154 @@
         <v>19</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30">
+      <c r="A67" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="2" t="s">
+    <row r="69" spans="1:3">
+      <c r="A69" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="45">
-      <c r="A68" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B68" s="2" t="s">
+    <row r="70" spans="1:3" ht="45">
+      <c r="A70" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="30">
-      <c r="A69" s="2" t="s">
+    <row r="71" spans="1:3" ht="30">
+      <c r="A71" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="30">
-      <c r="A70" s="2" t="s">
+    <row r="72" spans="1:3" ht="30">
+      <c r="A72" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="30">
-      <c r="A74" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="B74" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="30">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="30">
       <c r="A76" s="2" t="s">
-        <v>22</v>
+        <v>152</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>103</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="30">
       <c r="A77" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="45">
+        <v>105</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="30">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="45">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="30">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="45">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="30">
@@ -2173,10 +2224,10 @@
         <v>22</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="30">
@@ -2184,10 +2235,10 @@
         <v>22</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="30">
@@ -2195,64 +2246,76 @@
         <v>22</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="30">
       <c r="A85" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="30">
+      <c r="A86" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="30">
+      <c r="A87" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="30">
+      <c r="A88" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="45">
-      <c r="A86" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B86" s="2" t="s">
+    <row r="89" spans="1:3" ht="45">
+      <c r="A89" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B87" s="2" t="s">
+    <row r="90" spans="1:3" ht="45">
+      <c r="A90" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>130</v>
+      <c r="C90" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2260,15 +2323,15 @@
         <v>151</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="2" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2276,96 +2339,169 @@
         <v>150</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="30">
-      <c r="A94" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="30">
-      <c r="A95" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="45">
-      <c r="A96" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" ht="30">
       <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="30">
       <c r="A98" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+        <v>135</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="45">
       <c r="A99" s="2" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>155</v>
+        <v>139</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="2" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="2" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>157</v>
       </c>
     </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="30">
+      <c r="A106" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="30">
+      <c r="A107" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C101">
+  <autoFilter ref="A1:C104">
     <filterColumn colId="0"/>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
@@ -2374,48 +2510,55 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C44" r:id="rId3"/>
-    <hyperlink ref="C43" r:id="rId4"/>
-    <hyperlink ref="C47" r:id="rId5"/>
-    <hyperlink ref="C14" r:id="rId6"/>
+    <hyperlink ref="C45" r:id="rId3"/>
+    <hyperlink ref="C44" r:id="rId4"/>
+    <hyperlink ref="C48" r:id="rId5"/>
+    <hyperlink ref="C15" r:id="rId6"/>
     <hyperlink ref="C13" r:id="rId7"/>
-    <hyperlink ref="C51" r:id="rId8"/>
-    <hyperlink ref="C52" r:id="rId9"/>
-    <hyperlink ref="C53" r:id="rId10"/>
-    <hyperlink ref="C57" r:id="rId11"/>
-    <hyperlink ref="C62" r:id="rId12"/>
-    <hyperlink ref="C68" r:id="rId13"/>
-    <hyperlink ref="C69" r:id="rId14"/>
-    <hyperlink ref="C70" r:id="rId15"/>
-    <hyperlink ref="C65" r:id="rId16"/>
-    <hyperlink ref="C71" r:id="rId17"/>
-    <hyperlink ref="C74" r:id="rId18"/>
-    <hyperlink ref="C75" r:id="rId19"/>
-    <hyperlink ref="C79" r:id="rId20"/>
-    <hyperlink ref="C45" r:id="rId21"/>
-    <hyperlink ref="C78" r:id="rId22"/>
-    <hyperlink ref="C80" r:id="rId23"/>
-    <hyperlink ref="C81" r:id="rId24"/>
-    <hyperlink ref="C82" r:id="rId25"/>
-    <hyperlink ref="C83" r:id="rId26"/>
-    <hyperlink ref="C84" r:id="rId27"/>
+    <hyperlink ref="C52" r:id="rId8"/>
+    <hyperlink ref="C53" r:id="rId9"/>
+    <hyperlink ref="C54" r:id="rId10"/>
+    <hyperlink ref="C59" r:id="rId11"/>
+    <hyperlink ref="C64" r:id="rId12"/>
+    <hyperlink ref="C70" r:id="rId13"/>
+    <hyperlink ref="C71" r:id="rId14"/>
+    <hyperlink ref="C72" r:id="rId15"/>
+    <hyperlink ref="C67" r:id="rId16"/>
+    <hyperlink ref="C73" r:id="rId17"/>
+    <hyperlink ref="C76" r:id="rId18"/>
+    <hyperlink ref="C77" r:id="rId19"/>
+    <hyperlink ref="C81" r:id="rId20"/>
+    <hyperlink ref="C46" r:id="rId21"/>
+    <hyperlink ref="C80" r:id="rId22"/>
+    <hyperlink ref="C82" r:id="rId23"/>
+    <hyperlink ref="C84" r:id="rId24"/>
+    <hyperlink ref="C85" r:id="rId25"/>
+    <hyperlink ref="C86" r:id="rId26"/>
+    <hyperlink ref="C87" r:id="rId27"/>
     <hyperlink ref="C11" r:id="rId28"/>
     <hyperlink ref="C10" r:id="rId29"/>
-    <hyperlink ref="C85" r:id="rId30"/>
-    <hyperlink ref="C95" r:id="rId31"/>
-    <hyperlink ref="C19" r:id="rId32"/>
-    <hyperlink ref="C24" r:id="rId33"/>
-    <hyperlink ref="C34" r:id="rId34"/>
-    <hyperlink ref="C61" r:id="rId35"/>
-    <hyperlink ref="C94" r:id="rId36"/>
-    <hyperlink ref="C58" r:id="rId37"/>
-    <hyperlink ref="C99" r:id="rId38"/>
-    <hyperlink ref="C100" r:id="rId39"/>
-    <hyperlink ref="C101" r:id="rId40"/>
-    <hyperlink ref="C86" r:id="rId41"/>
-    <hyperlink ref="C97" r:id="rId42"/>
+    <hyperlink ref="C88" r:id="rId30"/>
+    <hyperlink ref="C98" r:id="rId31"/>
+    <hyperlink ref="C20" r:id="rId32"/>
+    <hyperlink ref="C25" r:id="rId33"/>
+    <hyperlink ref="C35" r:id="rId34"/>
+    <hyperlink ref="C63" r:id="rId35"/>
+    <hyperlink ref="C97" r:id="rId36"/>
+    <hyperlink ref="C60" r:id="rId37"/>
+    <hyperlink ref="C102" r:id="rId38"/>
+    <hyperlink ref="C103" r:id="rId39"/>
+    <hyperlink ref="C104" r:id="rId40"/>
+    <hyperlink ref="C89" r:id="rId41"/>
+    <hyperlink ref="C100" r:id="rId42"/>
+    <hyperlink ref="C105" r:id="rId43"/>
+    <hyperlink ref="C90" r:id="rId44"/>
+    <hyperlink ref="C83" r:id="rId45"/>
+    <hyperlink ref="C106" r:id="rId46"/>
+    <hyperlink ref="C14" r:id="rId47"/>
+    <hyperlink ref="C107" r:id="rId48"/>
+    <hyperlink ref="C38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new core java questions and example of serialization
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="181">
   <si>
     <t>Topic</t>
   </si>
@@ -556,6 +556,12 @@
   </si>
   <si>
     <t>Let say we locked one object thinking to so some operation and before starting the operation we found the condition is not satisfying to do that operation so as we know wait() method releases the lock. If we do not hold any lock then how can we release the lock? And if that condition satisfies then we cand easily do that operation and release the lock and notify other waiting threads that I am done with the operation now you can take a lock by calling notify() or notifyAll() method.</t>
+  </si>
+  <si>
+    <t>What is the purpose of serial version UID?</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/285793/what-is-a-serialversionuid-and-why-should-i-use-it</t>
   </si>
 </sst>
 </file>
@@ -1430,11 +1436,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2498,6 +2504,17 @@
       </c>
       <c r="B109" s="2" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="30">
+      <c r="A110" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2556,9 +2573,10 @@
     <hyperlink ref="C106" r:id="rId46"/>
     <hyperlink ref="C14" r:id="rId47"/>
     <hyperlink ref="C107" r:id="rId48"/>
-    <hyperlink ref="C38"/>
+    <hyperlink ref="C38" display="https://stackoverflow.com/questions/17840397/concept-behind-putting-wait-notify-methods-in-object-class#:~:text=wait%20%2D%20wait%20method%20tells%20the,monitor%20and%20go%20to%20sleep.&amp;text=That's%20one%20reason%20why%20these,waiting%20on%20the%20Object'"/>
+    <hyperlink ref="C110" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId49"/>
+  <pageSetup orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more inteview questions
</commit_message>
<xml_diff>
--- a/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
+++ b/src/com/corejava/practice/interview/InterviewQuestions (Core Java).xlsx
@@ -10,14 +10,14 @@
     <sheet name="CoreJavaTopicsOrQuestions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CoreJavaTopicsOrQuestions!$A$1:$C$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CoreJavaTopicsOrQuestions!$A$1:$C$118</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="202">
   <si>
     <t>Topic</t>
   </si>
@@ -419,9 +419,6 @@
     <t>What is method reference in java?</t>
   </si>
   <si>
-    <t>Difference between lambda expression and anonymous inner class</t>
-  </si>
-  <si>
     <t>What is the difference between PermGenSpace and MetaSpace?</t>
   </si>
   <si>
@@ -453,9 +450,6 @@
   </si>
   <si>
     <t>https://howtodoinjava.com/java/multi-threading/executor-framework-tutorial/</t>
-  </si>
-  <si>
-    <t>http://karunsubramanian.com/websphere/one-important-change-in-memory-management-in-java-8/</t>
   </si>
   <si>
     <t>Size of the boolean in java is virtual machine dependent.
@@ -504,9 +498,6 @@
     <t>JVM architechture.</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=dncpVFP1JeQ</t>
-  </si>
-  <si>
     <t>Exception</t>
   </si>
   <si>
@@ -571,6 +562,70 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/602079/java-object-serialization-performance-tips</t>
+  </si>
+  <si>
+    <t>Generics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why List&lt;String&gt; is not acceptable as List&lt;Object&gt;? </t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/22144671/why-liststring-is-not-acceptable-as-listobject</t>
+  </si>
+  <si>
+    <t>What are the restrictions in using generic type that is declared in a class declaration?</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/generics/restrictions.html</t>
+  </si>
+  <si>
+    <t>What is the difference between ? and Object in Java generics?</t>
+  </si>
+  <si>
+    <t>How can we restrict Generics to a subclass of particular class?</t>
+  </si>
+  <si>
+    <t>What is type erasure?</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/generics/erasure.html</t>
+  </si>
+  <si>
+    <t>What is bridge method?</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/generics/bridgeMethods.html</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dncpVFP1JeQ
+https://javapapers.com/core-java/java-jvm-memory-types/</t>
+  </si>
+  <si>
+    <t>How Garbage collection works?</t>
+  </si>
+  <si>
+    <t>https://www.oracle.com/webfolder/technetwork/tutorials/obe/java/gc01/index.html.</t>
+  </si>
+  <si>
+    <t>https://dzone.com/articles/java-8-permgen-metaspace</t>
+  </si>
+  <si>
+    <t>What is Inheritance?</t>
+  </si>
+  <si>
+    <t>What is polymorphism?</t>
+  </si>
+  <si>
+    <t>Can we throw exception from constructor?</t>
+  </si>
+  <si>
+    <t>What is the output of System.out.println(10.0/-0);</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>What are the type of polymorphism?</t>
   </si>
 </sst>
 </file>
@@ -1445,11 +1500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1517,7 +1572,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -1528,7 +1583,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -1539,7 +1594,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -1580,7 +1635,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
@@ -1588,7 +1643,7 @@
     </row>
     <row r="13" spans="1:3" ht="30">
       <c r="A13" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1599,18 +1654,18 @@
     </row>
     <row r="14" spans="1:3" ht="30">
       <c r="A14" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30">
       <c r="A15" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>18</v>
@@ -1629,7 +1684,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>59</v>
@@ -1637,7 +1692,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
@@ -1659,12 +1714,12 @@
         <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>26</v>
@@ -1672,13 +1727,13 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1691,7 +1746,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>28</v>
@@ -1702,18 +1757,18 @@
     </row>
     <row r="25" spans="1:3" ht="30">
       <c r="A25" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>30</v>
@@ -1721,7 +1776,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>31</v>
@@ -1794,7 +1849,7 @@
         <v>40</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1821,7 +1876,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="135">
@@ -1832,7 +1887,7 @@
         <v>44</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1880,7 +1935,7 @@
     </row>
     <row r="45" spans="1:3" ht="30">
       <c r="A45" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>52</v>
@@ -2008,12 +2063,12 @@
         <v>95</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="30">
       <c r="A59" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>75</v>
@@ -2030,7 +2085,7 @@
         <v>78</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2057,7 +2112,7 @@
         <v>80</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="45">
@@ -2089,7 +2144,7 @@
     </row>
     <row r="67" spans="1:3" ht="30">
       <c r="A67" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>97</v>
@@ -2149,7 +2204,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>99</v>
@@ -2176,7 +2231,7 @@
     </row>
     <row r="76" spans="1:3" ht="30">
       <c r="A76" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>103</v>
@@ -2250,10 +2305,10 @@
         <v>22</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="30">
@@ -2308,7 +2363,7 @@
         <v>125</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="45">
@@ -2319,7 +2374,7 @@
         <v>126</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="45">
@@ -2330,12 +2385,12 @@
         <v>127</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>128</v>
@@ -2343,7 +2398,7 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>129</v>
@@ -2351,7 +2406,7 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>130</v>
@@ -2359,7 +2414,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>131</v>
@@ -2375,62 +2430,65 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="2" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>133</v>
       </c>
+      <c r="C96" s="3" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="97" spans="1:3" ht="30">
       <c r="A97" s="2" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="30">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="45">
       <c r="A98" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="45">
       <c r="A99" s="2" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>146</v>
+        <v>158</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="2" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="2" t="s">
-        <v>147</v>
+        <v>19</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2452,7 +2510,7 @@
         <v>156</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2460,43 +2518,40 @@
         <v>19</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="30">
       <c r="A105" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="30">
       <c r="A106" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="30">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2504,39 +2559,42 @@
         <v>22</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="30">
       <c r="A109" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="30">
+        <v>176</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="30">
       <c r="A111" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="30">
       <c r="A112" s="2" t="s">
-        <v>11</v>
+        <v>181</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>182</v>
@@ -2545,8 +2603,111 @@
         <v>183</v>
       </c>
     </row>
+    <row r="113" spans="1:3" ht="30">
+      <c r="A113" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="30">
+      <c r="A116" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="30">
+      <c r="A117" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="30">
+      <c r="A118" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C104">
+  <autoFilter ref="A1:C118">
     <filterColumn colId="0"/>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
@@ -2583,29 +2744,34 @@
     <hyperlink ref="C11" r:id="rId28"/>
     <hyperlink ref="C10" r:id="rId29"/>
     <hyperlink ref="C88" r:id="rId30"/>
-    <hyperlink ref="C98" r:id="rId31"/>
+    <hyperlink ref="C97" r:id="rId31"/>
     <hyperlink ref="C20" r:id="rId32"/>
     <hyperlink ref="C25" r:id="rId33"/>
     <hyperlink ref="C35" r:id="rId34"/>
     <hyperlink ref="C63" r:id="rId35"/>
-    <hyperlink ref="C97" r:id="rId36"/>
+    <hyperlink ref="C96" r:id="rId36"/>
     <hyperlink ref="C60" r:id="rId37"/>
-    <hyperlink ref="C102" r:id="rId38"/>
-    <hyperlink ref="C103" r:id="rId39"/>
-    <hyperlink ref="C104" r:id="rId40"/>
+    <hyperlink ref="C101" r:id="rId38"/>
+    <hyperlink ref="C102" r:id="rId39"/>
+    <hyperlink ref="C103" r:id="rId40"/>
     <hyperlink ref="C89" r:id="rId41"/>
-    <hyperlink ref="C100" r:id="rId42"/>
-    <hyperlink ref="C105" r:id="rId43"/>
+    <hyperlink ref="C99" r:id="rId42" display="https://www.youtube.com/watch?v=dncpVFP1JeQ"/>
+    <hyperlink ref="C104" r:id="rId43"/>
     <hyperlink ref="C90" r:id="rId44"/>
     <hyperlink ref="C83" r:id="rId45"/>
-    <hyperlink ref="C106" r:id="rId46"/>
+    <hyperlink ref="C105" r:id="rId46"/>
     <hyperlink ref="C14" r:id="rId47"/>
-    <hyperlink ref="C107" r:id="rId48"/>
+    <hyperlink ref="C106" r:id="rId48"/>
     <hyperlink ref="C38" display="https://stackoverflow.com/questions/17840397/concept-behind-putting-wait-notify-methods-in-object-class#:~:text=wait%20%2D%20wait%20method%20tells%20the,monitor%20and%20go%20to%20sleep.&amp;text=That's%20one%20reason%20why%20these,waiting%20on%20the%20Object'"/>
-    <hyperlink ref="C110" r:id="rId49"/>
-    <hyperlink ref="C112" r:id="rId50"/>
+    <hyperlink ref="C109" r:id="rId49"/>
+    <hyperlink ref="C111" r:id="rId50"/>
+    <hyperlink ref="C112" r:id="rId51"/>
+    <hyperlink ref="C113" r:id="rId52"/>
+    <hyperlink ref="C116" r:id="rId53"/>
+    <hyperlink ref="C117" r:id="rId54"/>
+    <hyperlink ref="C118" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId51"/>
+  <pageSetup orientation="portrait" r:id="rId56"/>
 </worksheet>
 </file>
</xml_diff>